<commit_message>
Edited ER_diagram, Schemas and Normalization table
</commit_message>
<xml_diff>
--- a/ASSETS/Нормалізація таблиць.xlsx
+++ b/ASSETS/Нормалізація таблиць.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>Номер_замовлення</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>ID_клієнта</t>
+  </si>
+  <si>
+    <t>Таблиця "Деталі замовлення"</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,6 +246,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D51" activeCellId="1" sqref="F47 D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -679,7 +700,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
@@ -699,7 +720,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>21</v>
@@ -719,7 +740,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>20</v>
@@ -771,7 +792,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>20</v>
@@ -782,7 +803,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
@@ -793,7 +814,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>20</v>
@@ -837,7 +858,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>14</v>
@@ -851,7 +872,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>15</v>
@@ -865,7 +886,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>16</v>
@@ -969,18 +990,18 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -989,15 +1010,11 @@
       <c r="C46" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D46" s="14"/>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="4">
+      <c r="A47" s="16">
         <v>101</v>
       </c>
       <c r="B47" s="13">
@@ -1006,16 +1023,12 @@
       <c r="C47" s="11">
         <v>100001</v>
       </c>
-      <c r="D47" s="4">
-        <v>3</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="4">
-        <v>101</v>
+      <c r="A48" s="16">
+        <v>102</v>
       </c>
       <c r="B48" s="13">
         <v>1</v>
@@ -1023,16 +1036,12 @@
       <c r="C48" s="11">
         <v>100002</v>
       </c>
-      <c r="D48" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="4">
-        <v>102</v>
+      <c r="A49" s="16">
+        <v>103</v>
       </c>
       <c r="B49" s="13">
         <v>2</v>
@@ -1040,16 +1049,12 @@
       <c r="C49" s="11">
         <v>100003</v>
       </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="4">
-        <v>103</v>
+      <c r="A50" s="16">
+        <v>104</v>
       </c>
       <c r="B50" s="13">
         <v>3</v>
@@ -1057,15 +1062,82 @@
       <c r="C50" s="11">
         <v>100002</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="9"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="16">
+        <v>101</v>
+      </c>
+      <c r="B54" s="4">
+        <v>3</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="16">
+        <v>102</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="16">
+        <v>103</v>
+      </c>
+      <c r="B56" s="4">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="16">
+        <v>104</v>
+      </c>
+      <c r="B57" s="4">
         <v>4</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E51" s="8"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>